<commit_message>
Work more on Storytelling with Data
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1985ABD8-20C9-4F4B-908A-2F5FC1AB6BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA69D57-C646-4F67-B6E4-2087F47CE2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Survey item E</t>
+  </si>
+  <si>
+    <t>There really are just three options: Disagree, Neutral, Agree.</t>
+  </si>
+  <si>
+    <t>https://medium.com/nightingale/seven-different-ways-to-display-likert-scale-data-d0c1c9a9ad59</t>
+  </si>
+  <si>
+    <t>Try the diverging bar chart</t>
   </si>
 </sst>
 </file>
@@ -4774,10 +4783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4962,22 +4971,34 @@
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added two approaches to investigate
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781CD059-5667-4F36-9107-7CC28E528E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676A5412-D9F1-4251-903A-60761FF96C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="444" yWindow="180" windowWidth="19248" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="what are your thoughts on this" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>https://mbounthavong.com/blog/2019/5/16/communicating-data-effectively-with-data-visualization-part-15-divergent-stacked-bar-chart-for-likert-scales</t>
+  </si>
+  <si>
+    <t>I need to try both horizontal and vertical approaches</t>
   </si>
 </sst>
 </file>
@@ -4794,8 +4797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5024,7 +5027,11 @@
       </c>
     </row>
     <row r="36" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="38" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Looking at pie charts
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676A5412-D9F1-4251-903A-60761FF96C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFDAAC9-E934-48DC-8E08-586709914068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="444" yWindow="180" windowWidth="19248" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>I need to try both horizontal and vertical approaches</t>
+  </si>
+  <si>
+    <t>pie charts are also a possibility.</t>
   </si>
 </sst>
 </file>
@@ -4797,8 +4800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5033,7 +5036,11 @@
       </c>
     </row>
     <row r="38" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="40" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Putting down more thoughts on options
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFDAAC9-E934-48DC-8E08-586709914068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF21D90D-8F06-4446-9BD9-67629ECED973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="444" yWindow="180" windowWidth="19248" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>pie charts are also a possibility.</t>
+  </si>
+  <si>
+    <t>Consider more narrative options</t>
   </si>
 </sst>
 </file>
@@ -4800,8 +4803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5042,7 +5045,11 @@
       </c>
     </row>
     <row r="40" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="42" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on how to handle neutral
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF21D90D-8F06-4446-9BD9-67629ECED973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B96B5F-5B8D-4EE9-AB69-F1C3C9B2A071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="444" yWindow="180" windowWidth="19248" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Consider more narrative options</t>
+  </si>
+  <si>
+    <t>The problem for me is the neutral.</t>
+  </si>
+  <si>
+    <t>I don't know how to include that.</t>
   </si>
 </sst>
 </file>
@@ -4803,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5051,8 +5057,16 @@
       </c>
     </row>
     <row r="42" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="45" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More comments on project
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26421"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B96B5F-5B8D-4EE9-AB69-F1C3C9B2A071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F56F54B-5FDA-4217-867B-AA424FA7CF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="180" windowWidth="19248" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="what are your thoughts on this" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>I don't know how to include that.</t>
+  </si>
+  <si>
+    <t>A pie chart might not be that bad.</t>
   </si>
 </sst>
 </file>
@@ -4809,8 +4812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5068,7 +5071,11 @@
       </c>
     </row>
     <row r="45" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="47" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
I am still struggling with thw SWD April challenge
</commit_message>
<xml_diff>
--- a/SWD_EX42.xlsx
+++ b/SWD_EX42.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F56F54B-5FDA-4217-867B-AA424FA7CF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1879BCEE-5BFC-4FDA-8F97-2060087A27CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>DATA TO GRAPH</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>A pie chart might not be that bad.</t>
+  </si>
+  <si>
+    <t>I have not resolved how to handle three items. Only the pie chart seems simple. I hate to use that.</t>
   </si>
 </sst>
 </file>
@@ -4812,8 +4815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="D26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5077,7 +5080,11 @@
       </c>
     </row>
     <row r="47" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>